<commit_message>
-dab documentation -bom Mainboard.b#1 -small changes pcb
</commit_message>
<xml_diff>
--- a/pcb/RGBClock/BOM-Farnell-Digikey.xlsx
+++ b/pcb/RGBClock/BOM-Farnell-Digikey.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="10824" windowHeight="8016" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Proto" sheetId="1" r:id="rId1"/>
@@ -14,16 +14,18 @@
     <sheet name="iPrototype" sheetId="6" r:id="rId5"/>
     <sheet name="Digikey" sheetId="5" r:id="rId6"/>
     <sheet name="MB-Farnell-Basket" sheetId="7" r:id="rId7"/>
-    <sheet name="DB-Farnell-Basket" sheetId="8" r:id="rId8"/>
-    <sheet name="LD-Farnell-Basket" sheetId="9" r:id="rId9"/>
-    <sheet name="Basket" sheetId="10" r:id="rId10"/>
+    <sheet name="DAB+MB Farnell" sheetId="11" r:id="rId8"/>
+    <sheet name="DAB+ Test" sheetId="12" r:id="rId9"/>
+    <sheet name="DB-Farnell-Basket" sheetId="8" r:id="rId10"/>
+    <sheet name="LD-Farnell-Basket" sheetId="9" r:id="rId11"/>
+    <sheet name="Basket" sheetId="10" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="basket_1" localSheetId="6">'MB-Farnell-Basket'!$A$1:$J$56</definedName>
-    <definedName name="basketdb" localSheetId="7">'DB-Farnell-Basket'!$A$1:$J$51</definedName>
-    <definedName name="basketld" localSheetId="8">'LD-Farnell-Basket'!$A$1:$J$5</definedName>
+    <definedName name="basketdb" localSheetId="9">'DB-Farnell-Basket'!$A$1:$J$51</definedName>
+    <definedName name="basketld" localSheetId="10">'LD-Farnell-Basket'!$A$1:$J$5</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -81,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="368">
   <si>
     <t>Toch button</t>
   </si>
@@ -1044,13 +1046,154 @@
   </si>
   <si>
     <t>dd</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>C1,C6,C7</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>C3,C4</t>
+  </si>
+  <si>
+    <t>D6-D7</t>
+  </si>
+  <si>
+    <t>LM2675M-5.0</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>LT1763CS8-1.5</t>
+  </si>
+  <si>
+    <t>D2,D3</t>
+  </si>
+  <si>
+    <t>3.3K</t>
+  </si>
+  <si>
+    <t>R2,R3</t>
+  </si>
+  <si>
+    <t>MAX6369KA</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>33pF</t>
+  </si>
+  <si>
+    <t>U$3</t>
+  </si>
+  <si>
+    <t>ESD Prot Low Cap</t>
+  </si>
+  <si>
+    <t>C9,C10,C16,C17</t>
+  </si>
+  <si>
+    <t>18nh</t>
+  </si>
+  <si>
+    <t>U$1</t>
+  </si>
+  <si>
+    <t>120nH</t>
+  </si>
+  <si>
+    <t>U$4</t>
+  </si>
+  <si>
+    <t>22nH</t>
+  </si>
+  <si>
+    <t>U$5</t>
+  </si>
+  <si>
+    <t>8.2pF</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>DRV612PW</t>
+  </si>
+  <si>
+    <t>C13, C22,C27,C28,C23,C19,C20,C21</t>
+  </si>
+  <si>
+    <t>C11,C12,C24,C25,C26,C29</t>
+  </si>
+  <si>
+    <t>R8,R9,R10,R11</t>
+  </si>
+  <si>
+    <t>47k</t>
+  </si>
+  <si>
+    <t>R6,R7</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>1469923</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>2930572</t>
+  </si>
+  <si>
+    <t>SI4684</t>
+  </si>
+  <si>
+    <t>U$6</t>
+  </si>
+  <si>
+    <t>2849437</t>
+  </si>
+  <si>
+    <t>U$2</t>
+  </si>
+  <si>
+    <t>19.2Mhz</t>
+  </si>
+  <si>
+    <t>X3,X4</t>
+  </si>
+  <si>
+    <t>2675146</t>
+  </si>
+  <si>
+    <t>D8,D9,D10,D11</t>
+  </si>
+  <si>
+    <t>1N4148 </t>
+  </si>
+  <si>
+    <t>2695042</t>
+  </si>
+  <si>
+    <t>1658877</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1096,6 +1239,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1118,7 +1267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1132,6 +1281,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1142,6 +1293,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1202,7 +1356,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1237,7 +1391,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1452,13 +1606,13 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>4</v>
       </c>
@@ -1469,7 +1623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1480,7 +1634,7 @@
         <v>8.4499999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1497,7 +1651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1514,7 +1668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1531,7 +1685,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1551,7 +1705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1565,7 +1719,7 @@
         <v>2.2599999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1579,17 +1733,17 @@
         <v>2.99</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1606,7 +1760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1617,7 +1771,7 @@
         <v>1657931</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1644,18 +1798,1146 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2317402</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3">
+        <v>0.99</v>
+      </c>
+      <c r="J3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2309036</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I4">
+        <v>0.78</v>
+      </c>
+      <c r="J4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1759246</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" t="s">
+        <v>147</v>
+      </c>
+      <c r="I6">
+        <v>0.13</v>
+      </c>
+      <c r="J6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1286784</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" t="s">
+        <v>156</v>
+      </c>
+      <c r="H7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I7">
+        <v>7.3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>1527537</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G9" t="s">
+        <v>159</v>
+      </c>
+      <c r="H9" t="s">
+        <v>147</v>
+      </c>
+      <c r="I9">
+        <v>0.41</v>
+      </c>
+      <c r="J9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>1527471</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H10" t="s">
+        <v>147</v>
+      </c>
+      <c r="I10">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>2309029</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" t="s">
+        <v>165</v>
+      </c>
+      <c r="H12" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12">
+        <v>0.45</v>
+      </c>
+      <c r="J12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>1759223</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" t="s">
+        <v>168</v>
+      </c>
+      <c r="H13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13">
+        <v>0.23</v>
+      </c>
+      <c r="J13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>1759156</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" t="s">
+        <v>170</v>
+      </c>
+      <c r="F14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" t="s">
+        <v>171</v>
+      </c>
+      <c r="H14" t="s">
+        <v>147</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>1135383</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F15" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" t="s">
+        <v>175</v>
+      </c>
+      <c r="H15" t="s">
+        <v>147</v>
+      </c>
+      <c r="I15">
+        <v>2.11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>8906068</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" t="s">
+        <v>177</v>
+      </c>
+      <c r="F16" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" t="s">
+        <v>147</v>
+      </c>
+      <c r="I16">
+        <v>14.14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>2115321</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>179</v>
+      </c>
+      <c r="E18" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G18" t="s">
+        <v>181</v>
+      </c>
+      <c r="H18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I18">
+        <v>0.73</v>
+      </c>
+      <c r="J18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>2329934</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>182</v>
+      </c>
+      <c r="E19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" t="s">
+        <v>184</v>
+      </c>
+      <c r="H19" t="s">
+        <v>147</v>
+      </c>
+      <c r="I19">
+        <v>0.32</v>
+      </c>
+      <c r="J19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>1854074</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" t="s">
+        <v>186</v>
+      </c>
+      <c r="F21" t="s">
+        <v>145</v>
+      </c>
+      <c r="G21" t="s">
+        <v>187</v>
+      </c>
+      <c r="H21" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21">
+        <v>2.97</v>
+      </c>
+      <c r="J21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>2341911</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22" t="s">
+        <v>189</v>
+      </c>
+      <c r="F22" t="s">
+        <v>145</v>
+      </c>
+      <c r="G22" t="s">
+        <v>190</v>
+      </c>
+      <c r="H22" t="s">
+        <v>147</v>
+      </c>
+      <c r="I22">
+        <v>1.52</v>
+      </c>
+      <c r="J22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>16</v>
+      </c>
+      <c r="B24">
+        <v>1243244</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F24" t="s">
+        <v>145</v>
+      </c>
+      <c r="G24" t="s">
+        <v>193</v>
+      </c>
+      <c r="H24" t="s">
+        <v>147</v>
+      </c>
+      <c r="I24">
+        <v>5.36</v>
+      </c>
+      <c r="J24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>17</v>
+      </c>
+      <c r="B25">
+        <v>1332087</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>194</v>
+      </c>
+      <c r="E25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F25" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" t="s">
+        <v>196</v>
+      </c>
+      <c r="H25" t="s">
+        <v>147</v>
+      </c>
+      <c r="I25">
+        <v>2.91</v>
+      </c>
+      <c r="J25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>18</v>
+      </c>
+      <c r="B27">
+        <v>1207307</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>197</v>
+      </c>
+      <c r="E27" t="s">
+        <v>198</v>
+      </c>
+      <c r="F27" t="s">
+        <v>145</v>
+      </c>
+      <c r="G27" t="s">
+        <v>199</v>
+      </c>
+      <c r="H27" t="s">
+        <v>147</v>
+      </c>
+      <c r="I27">
+        <v>8.09</v>
+      </c>
+      <c r="J27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>19</v>
+      </c>
+      <c r="B28">
+        <v>1843876</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>200</v>
+      </c>
+      <c r="E28" t="s">
+        <v>201</v>
+      </c>
+      <c r="F28" t="s">
+        <v>145</v>
+      </c>
+      <c r="G28" t="s">
+        <v>202</v>
+      </c>
+      <c r="H28" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28">
+        <v>17.78</v>
+      </c>
+      <c r="J28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>1657931</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>203</v>
+      </c>
+      <c r="E29" t="s">
+        <v>204</v>
+      </c>
+      <c r="F29" t="s">
+        <v>145</v>
+      </c>
+      <c r="G29">
+        <v>0.76</v>
+      </c>
+      <c r="H29" t="s">
+        <v>147</v>
+      </c>
+      <c r="I29">
+        <f>G29*C29</f>
+        <v>1.52</v>
+      </c>
+      <c r="J29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>21</v>
+      </c>
+      <c r="B30">
+        <v>1892899</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>205</v>
+      </c>
+      <c r="E30" t="s">
+        <v>206</v>
+      </c>
+      <c r="F30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G30" t="s">
+        <v>207</v>
+      </c>
+      <c r="H30" t="s">
+        <v>147</v>
+      </c>
+      <c r="I30">
+        <v>0.66</v>
+      </c>
+      <c r="J30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>22</v>
+      </c>
+      <c r="B31">
+        <v>9101241</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>208</v>
+      </c>
+      <c r="E31" t="s">
+        <v>209</v>
+      </c>
+      <c r="F31" t="s">
+        <v>210</v>
+      </c>
+      <c r="G31" t="s">
+        <v>190</v>
+      </c>
+      <c r="H31" t="s">
+        <v>147</v>
+      </c>
+      <c r="I31">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="J31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>23</v>
+      </c>
+      <c r="B33">
+        <v>1636136</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" t="s">
+        <v>212</v>
+      </c>
+      <c r="F33" t="s">
+        <v>145</v>
+      </c>
+      <c r="G33" t="s">
+        <v>213</v>
+      </c>
+      <c r="H33" t="s">
+        <v>147</v>
+      </c>
+      <c r="I33">
+        <v>10.32</v>
+      </c>
+      <c r="J33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>24</v>
+      </c>
+      <c r="B34">
+        <v>1085264</v>
+      </c>
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>214</v>
+      </c>
+      <c r="E34" t="s">
+        <v>215</v>
+      </c>
+      <c r="F34" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" t="s">
+        <v>216</v>
+      </c>
+      <c r="H34" t="s">
+        <v>147</v>
+      </c>
+      <c r="I34">
+        <v>0.61</v>
+      </c>
+      <c r="J34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>25</v>
+      </c>
+      <c r="B36">
+        <v>1085266</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>217</v>
+      </c>
+      <c r="E36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F36" t="s">
+        <v>145</v>
+      </c>
+      <c r="G36" t="s">
+        <v>216</v>
+      </c>
+      <c r="H36" t="s">
+        <v>147</v>
+      </c>
+      <c r="I36">
+        <v>0.61</v>
+      </c>
+      <c r="J36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>26</v>
+      </c>
+      <c r="B37">
+        <v>1759252</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>219</v>
+      </c>
+      <c r="E37" t="s">
+        <v>220</v>
+      </c>
+      <c r="F37" t="s">
+        <v>145</v>
+      </c>
+      <c r="G37" t="s">
+        <v>221</v>
+      </c>
+      <c r="H37" t="s">
+        <v>147</v>
+      </c>
+      <c r="I37">
+        <v>0.17</v>
+      </c>
+      <c r="J37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>27</v>
+      </c>
+      <c r="B39">
+        <v>1563120</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>222</v>
+      </c>
+      <c r="E39" t="s">
+        <v>223</v>
+      </c>
+      <c r="F39" t="s">
+        <v>145</v>
+      </c>
+      <c r="G39" t="s">
+        <v>224</v>
+      </c>
+      <c r="H39" t="s">
+        <v>147</v>
+      </c>
+      <c r="I39">
+        <v>0.23</v>
+      </c>
+      <c r="J39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>28</v>
+      </c>
+      <c r="B40">
+        <v>1226888</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>225</v>
+      </c>
+      <c r="E40" t="s">
+        <v>226</v>
+      </c>
+      <c r="F40" t="s">
+        <v>145</v>
+      </c>
+      <c r="G40" t="s">
+        <v>227</v>
+      </c>
+      <c r="H40" t="s">
+        <v>147</v>
+      </c>
+      <c r="I40">
+        <v>4.41</v>
+      </c>
+      <c r="J40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>29</v>
+      </c>
+      <c r="B42">
+        <v>1103919</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>228</v>
+      </c>
+      <c r="E42" t="s">
+        <v>229</v>
+      </c>
+      <c r="F42" t="s">
+        <v>145</v>
+      </c>
+      <c r="G42" t="s">
+        <v>230</v>
+      </c>
+      <c r="H42" t="s">
+        <v>147</v>
+      </c>
+      <c r="I42">
+        <v>2.09</v>
+      </c>
+      <c r="J42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>30</v>
+      </c>
+      <c r="B43">
+        <v>5095487</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>309</v>
+      </c>
+      <c r="E43" t="s">
+        <v>310</v>
+      </c>
+      <c r="F43" t="s">
+        <v>311</v>
+      </c>
+      <c r="G43" t="s">
+        <v>312</v>
+      </c>
+      <c r="H43" t="s">
+        <v>147</v>
+      </c>
+      <c r="I43">
+        <v>21.81</v>
+      </c>
+      <c r="J43" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>305</v>
+      </c>
+      <c r="I46">
+        <f>SUM(I3:I45)</f>
+        <v>114.78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1892887</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" t="s">
+        <v>315</v>
+      </c>
+      <c r="F3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" t="s">
+        <v>316</v>
+      </c>
+      <c r="H3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3" t="s">
+        <v>317</v>
+      </c>
+      <c r="J3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>305</v>
+      </c>
+      <c r="I5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>2317402</v>
       </c>
@@ -1666,7 +2948,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1563202</v>
       </c>
@@ -1677,7 +2959,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9227946</v>
       </c>
@@ -1688,7 +2970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2333744</v>
       </c>
@@ -1699,7 +2981,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1754000</v>
       </c>
@@ -1710,7 +2992,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1135383</v>
       </c>
@@ -1721,7 +3003,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1759156</v>
       </c>
@@ -1732,7 +3014,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1740680</v>
       </c>
@@ -1743,7 +3025,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1758991</v>
       </c>
@@ -1754,7 +3036,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1758951</v>
       </c>
@@ -1765,7 +3047,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2341911</v>
       </c>
@@ -1776,7 +3058,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1652573</v>
       </c>
@@ -1787,7 +3069,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1319749</v>
       </c>
@@ -1798,7 +3080,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1379714</v>
       </c>
@@ -1809,7 +3091,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2115321</v>
       </c>
@@ -1820,7 +3102,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2329964</v>
       </c>
@@ -1831,7 +3113,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2329934</v>
       </c>
@@ -1842,7 +3124,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1243244</v>
       </c>
@@ -1853,7 +3135,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1563074</v>
       </c>
@@ -1864,7 +3146,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1703315</v>
       </c>
@@ -1875,7 +3157,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1652645</v>
       </c>
@@ -1886,7 +3168,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2164820</v>
       </c>
@@ -1897,7 +3179,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1650715</v>
       </c>
@@ -1908,7 +3190,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1463389</v>
       </c>
@@ -1919,7 +3201,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1332087</v>
       </c>
@@ -1930,7 +3212,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1141477</v>
       </c>
@@ -1941,7 +3223,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2068190</v>
       </c>
@@ -1952,7 +3234,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1612436</v>
       </c>
@@ -1963,7 +3245,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1177883</v>
       </c>
@@ -1974,7 +3256,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>636370</v>
       </c>
@@ -1985,7 +3267,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1518419</v>
       </c>
@@ -1996,7 +3278,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1550980</v>
       </c>
@@ -2007,7 +3289,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1103922</v>
       </c>
@@ -2018,7 +3300,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2102054</v>
       </c>
@@ -2029,7 +3311,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>2329534</v>
       </c>
@@ -2040,7 +3322,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>2112412</v>
       </c>
@@ -2051,7 +3333,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2317402</v>
       </c>
@@ -2062,7 +3344,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2309036</v>
       </c>
@@ -2073,7 +3355,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1759246</v>
       </c>
@@ -2084,7 +3366,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1286784</v>
       </c>
@@ -2095,7 +3377,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1527537</v>
       </c>
@@ -2106,7 +3388,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1527471</v>
       </c>
@@ -2117,7 +3399,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2309029</v>
       </c>
@@ -2128,7 +3410,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1759223</v>
       </c>
@@ -2139,7 +3421,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1759156</v>
       </c>
@@ -2150,7 +3432,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1135383</v>
       </c>
@@ -2161,7 +3443,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>8906068</v>
       </c>
@@ -2172,7 +3454,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>2115321</v>
       </c>
@@ -2183,7 +3465,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>2329934</v>
       </c>
@@ -2194,7 +3476,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1854074</v>
       </c>
@@ -2205,7 +3487,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2341911</v>
       </c>
@@ -2216,7 +3498,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1243244</v>
       </c>
@@ -2227,7 +3509,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1332087</v>
       </c>
@@ -2238,7 +3520,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1207307</v>
       </c>
@@ -2249,7 +3531,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1843876</v>
       </c>
@@ -2260,7 +3542,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1657931</v>
       </c>
@@ -2271,7 +3553,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1892899</v>
       </c>
@@ -2282,7 +3564,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>9101241</v>
       </c>
@@ -2293,7 +3575,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1636136</v>
       </c>
@@ -2304,7 +3586,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>1085264</v>
       </c>
@@ -2315,7 +3597,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>1085266</v>
       </c>
@@ -2326,7 +3608,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1759252</v>
       </c>
@@ -2337,7 +3619,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>1563120</v>
       </c>
@@ -2348,7 +3630,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>1226888</v>
       </c>
@@ -2359,7 +3641,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>1103919</v>
       </c>
@@ -2370,7 +3652,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>5095487</v>
       </c>
@@ -2381,7 +3663,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1892887</v>
       </c>
@@ -2401,19 +3683,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="5" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" style="5" customWidth="1"/>
     <col min="6" max="6" width="32" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="7" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2436,7 +3718,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2317402</v>
       </c>
@@ -2454,7 +3736,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1563202</v>
       </c>
@@ -3224,15 +4506,15 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="11.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -3845,15 +5127,15 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="25.33203125" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="25.28515625" style="5"/>
+    <col min="1" max="1" width="10.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="25.33203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -3916,12 +5198,12 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>105</v>
       </c>
@@ -3938,7 +5220,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>56549884</v>
       </c>
@@ -3970,14 +5252,14 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="5"/>
+    <col min="1" max="1" width="26.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="5"/>
     <col min="3" max="3" width="43" style="5" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="5"/>
-    <col min="6" max="6" width="21.7109375" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="4" max="5" width="9.109375" style="5"/>
+    <col min="6" max="6" width="21.6640625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4321,25 +5603,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B55" sqref="B3:J55"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>133</v>
       </c>
@@ -4371,7 +5653,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4403,7 +5685,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4435,7 +5717,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4467,7 +5749,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4499,7 +5781,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4531,7 +5813,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4563,7 +5845,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4595,7 +5877,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4627,7 +5909,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4659,7 +5941,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>14</v>
       </c>
@@ -4691,7 +5973,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>15</v>
       </c>
@@ -4723,7 +6005,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
@@ -4755,7 +6037,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17</v>
       </c>
@@ -4787,7 +6069,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>18</v>
       </c>
@@ -4819,7 +6101,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>19</v>
       </c>
@@ -4851,7 +6133,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>21</v>
       </c>
@@ -4883,7 +6165,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>22</v>
       </c>
@@ -4915,7 +6197,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>23</v>
       </c>
@@ -4947,7 +6229,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>24</v>
       </c>
@@ -4979,7 +6261,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>25</v>
       </c>
@@ -5011,7 +6293,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>26</v>
       </c>
@@ -5043,7 +6325,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>27</v>
       </c>
@@ -5075,7 +6357,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>28</v>
       </c>
@@ -5107,7 +6389,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>29</v>
       </c>
@@ -5139,7 +6421,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>31</v>
       </c>
@@ -5171,7 +6453,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>32</v>
       </c>
@@ -5203,7 +6485,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>34</v>
       </c>
@@ -5235,7 +6517,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>35</v>
       </c>
@@ -5267,7 +6549,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>36</v>
       </c>
@@ -5299,7 +6581,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>37</v>
       </c>
@@ -5331,7 +6613,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>38</v>
       </c>
@@ -5363,7 +6645,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>39</v>
       </c>
@@ -5395,7 +6677,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>40</v>
       </c>
@@ -5427,7 +6709,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>41</v>
       </c>
@@ -5459,7 +6741,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>42</v>
       </c>
@@ -5488,7 +6770,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B55">
         <v>2112412</v>
       </c>
@@ -5502,7 +6784,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H56" t="s">
         <v>305</v>
       </c>
@@ -5518,1128 +6800,1090 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>133</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>1469911</v>
+      </c>
+      <c r="C5" t="s">
+        <v>331</v>
+      </c>
+      <c r="D5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>1469929</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1563074</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1141477</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>355</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>2070445</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>321</v>
+      </c>
+      <c r="D12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>9227946</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>2070445</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>323</v>
+      </c>
+      <c r="D14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>1754000</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>1759156</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>317603</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>335</v>
+      </c>
+      <c r="D17" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>1650715</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>2332712</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>345</v>
+      </c>
+      <c r="D19" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>1658877</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>346</v>
+      </c>
+      <c r="D20" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>1612436</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>283</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>2317402</v>
       </c>
-      <c r="C3">
+      <c r="B26">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C26" t="s">
         <v>143</v>
       </c>
-      <c r="E3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I3">
-        <v>0.99</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="D26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>2341911</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>2341911</v>
+      </c>
+      <c r="B28">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>2309036</v>
-      </c>
-      <c r="C4">
+      <c r="C28" t="s">
+        <v>188</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>2115321</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>179</v>
+      </c>
+      <c r="D29" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>365</v>
+      </c>
+      <c r="D30" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>1865863</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>339</v>
+      </c>
+      <c r="D33" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>1748783</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>341</v>
+      </c>
+      <c r="D34" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>9527982</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>343</v>
+      </c>
+      <c r="D35" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>1636136</v>
+      </c>
+      <c r="B36">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G4" t="s">
-        <v>150</v>
-      </c>
-      <c r="H4" t="s">
-        <v>147</v>
-      </c>
-      <c r="I4">
-        <v>0.78</v>
-      </c>
-      <c r="J4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C36" t="s">
+        <v>211</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>1332087</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>194</v>
+      </c>
+      <c r="D39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>2519138</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>333</v>
+      </c>
+      <c r="D40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>9489746</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>326</v>
+      </c>
+      <c r="D41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>1379714</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>257</v>
+      </c>
+      <c r="D42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>1703315</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>263</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>8906068</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>176</v>
+      </c>
+      <c r="D44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>1135383</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>2102598</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>329</v>
+      </c>
+      <c r="D46" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>2164820</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>268</v>
+      </c>
+      <c r="D47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>1882273</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>347</v>
+      </c>
+      <c r="D48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>357</v>
+      </c>
+      <c r="D49" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>2368172</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51" t="s">
+        <v>337</v>
+      </c>
+      <c r="D51" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>2068190</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54" t="s">
+        <v>280</v>
+      </c>
+      <c r="D54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>1652573</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>251</v>
+      </c>
+      <c r="D56" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="10">
+        <v>1319749</v>
+      </c>
+      <c r="B57" s="5">
+        <v>1</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>361</v>
+      </c>
+      <c r="D58" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>1243244</v>
+      </c>
+      <c r="B59">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>1759246</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F6" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" t="s">
-        <v>153</v>
-      </c>
-      <c r="H6" t="s">
-        <v>147</v>
-      </c>
-      <c r="I6">
-        <v>0.13</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>1286784</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" t="s">
-        <v>155</v>
-      </c>
-      <c r="F7" t="s">
-        <v>145</v>
-      </c>
-      <c r="G7" t="s">
-        <v>156</v>
-      </c>
-      <c r="H7" t="s">
-        <v>147</v>
-      </c>
-      <c r="I7">
-        <v>7.3</v>
-      </c>
-      <c r="J7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>1527537</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>157</v>
-      </c>
-      <c r="E9" t="s">
-        <v>158</v>
-      </c>
-      <c r="F9" t="s">
-        <v>145</v>
-      </c>
-      <c r="G9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H9" t="s">
-        <v>147</v>
-      </c>
-      <c r="I9">
-        <v>0.41</v>
-      </c>
-      <c r="J9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>1527471</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>160</v>
-      </c>
-      <c r="E10" t="s">
-        <v>161</v>
-      </c>
-      <c r="F10" t="s">
-        <v>145</v>
-      </c>
-      <c r="G10" t="s">
-        <v>162</v>
-      </c>
-      <c r="H10" t="s">
-        <v>147</v>
-      </c>
-      <c r="I10">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="J10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>2309029</v>
-      </c>
-      <c r="C12">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>163</v>
-      </c>
-      <c r="E12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F12" t="s">
-        <v>145</v>
-      </c>
-      <c r="G12" t="s">
-        <v>165</v>
-      </c>
-      <c r="H12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I12">
-        <v>0.45</v>
-      </c>
-      <c r="J12" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>1759223</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E13" t="s">
-        <v>167</v>
-      </c>
-      <c r="F13" t="s">
-        <v>145</v>
-      </c>
-      <c r="G13" t="s">
-        <v>168</v>
-      </c>
-      <c r="H13" t="s">
-        <v>147</v>
-      </c>
-      <c r="I13">
-        <v>0.23</v>
-      </c>
-      <c r="J13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>1759156</v>
-      </c>
-      <c r="C14">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>169</v>
-      </c>
-      <c r="E14" t="s">
-        <v>170</v>
-      </c>
-      <c r="F14" t="s">
-        <v>145</v>
-      </c>
-      <c r="G14" t="s">
-        <v>171</v>
-      </c>
-      <c r="H14" t="s">
-        <v>147</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>1135383</v>
-      </c>
-      <c r="C15">
+      <c r="C59" t="s">
+        <v>191</v>
+      </c>
+      <c r="D59" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>636370</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>1103922</v>
+      </c>
+      <c r="B61">
         <v>2</v>
       </c>
-      <c r="D15" t="s">
-        <v>173</v>
-      </c>
-      <c r="E15" t="s">
-        <v>174</v>
-      </c>
-      <c r="F15" t="s">
-        <v>145</v>
-      </c>
-      <c r="G15" t="s">
-        <v>175</v>
-      </c>
-      <c r="H15" t="s">
-        <v>147</v>
-      </c>
-      <c r="I15">
-        <v>2.11</v>
-      </c>
-      <c r="J15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>8906068</v>
-      </c>
-      <c r="C16">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>176</v>
-      </c>
-      <c r="E16" t="s">
-        <v>177</v>
-      </c>
-      <c r="F16" t="s">
-        <v>145</v>
-      </c>
-      <c r="G16" t="s">
-        <v>178</v>
-      </c>
-      <c r="H16" t="s">
-        <v>147</v>
-      </c>
-      <c r="I16">
-        <v>14.14</v>
-      </c>
-      <c r="J16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>2115321</v>
-      </c>
-      <c r="C18">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>179</v>
-      </c>
-      <c r="E18" t="s">
-        <v>180</v>
-      </c>
-      <c r="F18" t="s">
-        <v>145</v>
-      </c>
-      <c r="G18" t="s">
-        <v>181</v>
-      </c>
-      <c r="H18" t="s">
-        <v>147</v>
-      </c>
-      <c r="I18">
-        <v>0.73</v>
-      </c>
-      <c r="J18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>13</v>
-      </c>
-      <c r="B19">
-        <v>2329934</v>
-      </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>182</v>
-      </c>
-      <c r="E19" t="s">
-        <v>183</v>
-      </c>
-      <c r="F19" t="s">
-        <v>145</v>
-      </c>
-      <c r="G19" t="s">
-        <v>184</v>
-      </c>
-      <c r="H19" t="s">
-        <v>147</v>
-      </c>
-      <c r="I19">
-        <v>0.32</v>
-      </c>
-      <c r="J19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>14</v>
-      </c>
-      <c r="B21">
-        <v>1854074</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>185</v>
-      </c>
-      <c r="E21" t="s">
-        <v>186</v>
-      </c>
-      <c r="F21" t="s">
-        <v>145</v>
-      </c>
-      <c r="G21" t="s">
-        <v>187</v>
-      </c>
-      <c r="H21" t="s">
-        <v>147</v>
-      </c>
-      <c r="I21">
-        <v>2.97</v>
-      </c>
-      <c r="J21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>15</v>
-      </c>
-      <c r="B22">
-        <v>2341911</v>
-      </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>188</v>
-      </c>
-      <c r="E22" t="s">
-        <v>189</v>
-      </c>
-      <c r="F22" t="s">
-        <v>145</v>
-      </c>
-      <c r="G22" t="s">
-        <v>190</v>
-      </c>
-      <c r="H22" t="s">
-        <v>147</v>
-      </c>
-      <c r="I22">
-        <v>1.52</v>
-      </c>
-      <c r="J22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>16</v>
-      </c>
-      <c r="B24">
-        <v>1243244</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>191</v>
-      </c>
-      <c r="E24" t="s">
-        <v>192</v>
-      </c>
-      <c r="F24" t="s">
-        <v>145</v>
-      </c>
-      <c r="G24" t="s">
-        <v>193</v>
-      </c>
-      <c r="H24" t="s">
-        <v>147</v>
-      </c>
-      <c r="I24">
-        <v>5.36</v>
-      </c>
-      <c r="J24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>17</v>
-      </c>
-      <c r="B25">
-        <v>1332087</v>
-      </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>194</v>
-      </c>
-      <c r="E25" t="s">
-        <v>195</v>
-      </c>
-      <c r="F25" t="s">
-        <v>145</v>
-      </c>
-      <c r="G25" t="s">
-        <v>196</v>
-      </c>
-      <c r="H25" t="s">
-        <v>147</v>
-      </c>
-      <c r="I25">
-        <v>2.91</v>
-      </c>
-      <c r="J25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>18</v>
-      </c>
-      <c r="B27">
-        <v>1207307</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>197</v>
-      </c>
-      <c r="E27" t="s">
-        <v>198</v>
-      </c>
-      <c r="F27" t="s">
-        <v>145</v>
-      </c>
-      <c r="G27" t="s">
-        <v>199</v>
-      </c>
-      <c r="H27" t="s">
-        <v>147</v>
-      </c>
-      <c r="I27">
-        <v>8.09</v>
-      </c>
-      <c r="J27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>19</v>
-      </c>
-      <c r="B28">
-        <v>1843876</v>
-      </c>
-      <c r="C28">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
-        <v>200</v>
-      </c>
-      <c r="E28" t="s">
-        <v>201</v>
-      </c>
-      <c r="F28" t="s">
-        <v>145</v>
-      </c>
-      <c r="G28" t="s">
-        <v>202</v>
-      </c>
-      <c r="H28" t="s">
-        <v>147</v>
-      </c>
-      <c r="I28">
-        <v>17.78</v>
-      </c>
-      <c r="J28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>20</v>
-      </c>
-      <c r="B29">
-        <v>1657931</v>
-      </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29" t="s">
-        <v>203</v>
-      </c>
-      <c r="E29" t="s">
-        <v>204</v>
-      </c>
-      <c r="F29" t="s">
-        <v>145</v>
-      </c>
-      <c r="G29">
-        <v>0.76</v>
-      </c>
-      <c r="H29" t="s">
-        <v>147</v>
-      </c>
-      <c r="I29">
-        <f>G29*C29</f>
-        <v>1.52</v>
-      </c>
-      <c r="J29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>21</v>
-      </c>
-      <c r="B30">
-        <v>1892899</v>
-      </c>
-      <c r="C30">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
-        <v>205</v>
-      </c>
-      <c r="E30" t="s">
-        <v>206</v>
-      </c>
-      <c r="F30" t="s">
-        <v>145</v>
-      </c>
-      <c r="G30" t="s">
-        <v>207</v>
-      </c>
-      <c r="H30" t="s">
-        <v>147</v>
-      </c>
-      <c r="I30">
-        <v>0.66</v>
-      </c>
-      <c r="J30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>22</v>
-      </c>
-      <c r="B31">
-        <v>9101241</v>
-      </c>
-      <c r="C31">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>208</v>
-      </c>
-      <c r="E31" t="s">
-        <v>209</v>
-      </c>
-      <c r="F31" t="s">
-        <v>210</v>
-      </c>
-      <c r="G31" t="s">
-        <v>190</v>
-      </c>
-      <c r="H31" t="s">
-        <v>147</v>
-      </c>
-      <c r="I31">
-        <v>4.5599999999999996</v>
-      </c>
-      <c r="J31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>23</v>
-      </c>
-      <c r="B33">
-        <v>1636136</v>
-      </c>
-      <c r="C33">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>211</v>
-      </c>
-      <c r="E33" t="s">
-        <v>212</v>
-      </c>
-      <c r="F33" t="s">
-        <v>145</v>
-      </c>
-      <c r="G33" t="s">
-        <v>213</v>
-      </c>
-      <c r="H33" t="s">
-        <v>147</v>
-      </c>
-      <c r="I33">
-        <v>10.32</v>
-      </c>
-      <c r="J33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>24</v>
-      </c>
-      <c r="B34">
-        <v>1085264</v>
-      </c>
-      <c r="C34">
-        <v>3</v>
-      </c>
-      <c r="D34" t="s">
-        <v>214</v>
-      </c>
-      <c r="E34" t="s">
-        <v>215</v>
-      </c>
-      <c r="F34" t="s">
-        <v>145</v>
-      </c>
-      <c r="G34" t="s">
-        <v>216</v>
-      </c>
-      <c r="H34" t="s">
-        <v>147</v>
-      </c>
-      <c r="I34">
-        <v>0.61</v>
-      </c>
-      <c r="J34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>25</v>
-      </c>
-      <c r="B36">
-        <v>1085266</v>
-      </c>
-      <c r="C36">
-        <v>3</v>
-      </c>
-      <c r="D36" t="s">
-        <v>217</v>
-      </c>
-      <c r="E36" t="s">
-        <v>218</v>
-      </c>
-      <c r="F36" t="s">
-        <v>145</v>
-      </c>
-      <c r="G36" t="s">
-        <v>216</v>
-      </c>
-      <c r="H36" t="s">
-        <v>147</v>
-      </c>
-      <c r="I36">
-        <v>0.61</v>
-      </c>
-      <c r="J36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>26</v>
-      </c>
-      <c r="B37">
-        <v>1759252</v>
-      </c>
-      <c r="C37">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
-        <v>219</v>
-      </c>
-      <c r="E37" t="s">
-        <v>220</v>
-      </c>
-      <c r="F37" t="s">
-        <v>145</v>
-      </c>
-      <c r="G37" t="s">
-        <v>221</v>
-      </c>
-      <c r="H37" t="s">
-        <v>147</v>
-      </c>
-      <c r="I37">
-        <v>0.17</v>
-      </c>
-      <c r="J37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>27</v>
-      </c>
-      <c r="B39">
-        <v>1563120</v>
-      </c>
-      <c r="C39">
-        <v>5</v>
-      </c>
-      <c r="D39" t="s">
-        <v>222</v>
-      </c>
-      <c r="E39" t="s">
-        <v>223</v>
-      </c>
-      <c r="F39" t="s">
-        <v>145</v>
-      </c>
-      <c r="G39" t="s">
-        <v>224</v>
-      </c>
-      <c r="H39" t="s">
-        <v>147</v>
-      </c>
-      <c r="I39">
-        <v>0.23</v>
-      </c>
-      <c r="J39" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>28</v>
-      </c>
-      <c r="B40">
-        <v>1226888</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s">
-        <v>225</v>
-      </c>
-      <c r="E40" t="s">
-        <v>226</v>
-      </c>
-      <c r="F40" t="s">
-        <v>145</v>
-      </c>
-      <c r="G40" t="s">
-        <v>227</v>
-      </c>
-      <c r="H40" t="s">
-        <v>147</v>
-      </c>
-      <c r="I40">
-        <v>4.41</v>
-      </c>
-      <c r="J40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>29</v>
-      </c>
-      <c r="B42">
-        <v>1103919</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s">
-        <v>228</v>
-      </c>
-      <c r="E42" t="s">
-        <v>229</v>
-      </c>
-      <c r="F42" t="s">
-        <v>145</v>
-      </c>
-      <c r="G42" t="s">
-        <v>230</v>
-      </c>
-      <c r="H42" t="s">
-        <v>147</v>
-      </c>
-      <c r="I42">
-        <v>2.09</v>
-      </c>
-      <c r="J42" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>30</v>
-      </c>
-      <c r="B43">
-        <v>5095487</v>
-      </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s">
-        <v>309</v>
-      </c>
-      <c r="E43" t="s">
-        <v>310</v>
-      </c>
-      <c r="F43" t="s">
-        <v>311</v>
-      </c>
-      <c r="G43" t="s">
-        <v>312</v>
-      </c>
-      <c r="H43" t="s">
-        <v>147</v>
-      </c>
-      <c r="I43">
-        <v>21.81</v>
-      </c>
-      <c r="J43" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H46" t="s">
-        <v>305</v>
-      </c>
-      <c r="I46">
-        <f>SUM(I3:I45)</f>
-        <v>114.78</v>
+      <c r="C61" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A14" r:id="rId1" tooltip="2070445" display="https://be.farnell.com/kemet/c0805c104k5racauto/cap-0-1-f-50v-10-x7r-0805/dp/2070445"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:XFD62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>133</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" t="s">
-        <v>141</v>
-      </c>
-      <c r="J1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1892887</v>
-      </c>
-      <c r="C3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1141477</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>355</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>2070445</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>321</v>
+      </c>
+      <c r="D12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>9227946</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>234</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>2070445</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>323</v>
+      </c>
+      <c r="D14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>1754000</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>1759156</v>
+      </c>
+      <c r="B16">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
-        <v>314</v>
-      </c>
-      <c r="E3" t="s">
-        <v>315</v>
-      </c>
-      <c r="F3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G3" t="s">
-        <v>316</v>
-      </c>
-      <c r="H3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I3" t="s">
-        <v>317</v>
-      </c>
-      <c r="J3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H5" t="s">
-        <v>305</v>
-      </c>
-      <c r="I5" t="s">
-        <v>317</v>
+      <c r="C16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D16" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>317603</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>335</v>
+      </c>
+      <c r="D17" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>1650715</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D18" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>2332712</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>345</v>
+      </c>
+      <c r="D19" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>346</v>
+      </c>
+      <c r="D20" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>1612436</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>283</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>2317402</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>1865863</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>339</v>
+      </c>
+      <c r="D29" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>1748783</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>341</v>
+      </c>
+      <c r="D30" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>9527982</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>343</v>
+      </c>
+      <c r="D31" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>1636136</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>211</v>
+      </c>
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>9489746</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>326</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>1703315</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>263</v>
+      </c>
+      <c r="D39" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>1135383</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>2102598</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>329</v>
+      </c>
+      <c r="D42" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>1882273</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>347</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
+        <v>357</v>
+      </c>
+      <c r="D45" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>2368172</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>337</v>
+      </c>
+      <c r="D47" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="10"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>361</v>
+      </c>
+      <c r="D52" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>1243244</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>191</v>
+      </c>
+      <c r="D53" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>636370</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1103922</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A14" r:id="rId1" tooltip="2070445" display="https://be.farnell.com/kemet/c0805c104k5racauto/cap-0-1-f-50v-10-x7r-0805/dp/2070445"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>